<commit_message>
Settings: Update Settings - General - Import
</commit_message>
<xml_diff>
--- a/src/wl_tests_files/wl_file_area/file_types/Excel Workbook.xlsx
+++ b/src/wl_tests_files/wl_file_area/file_types/Excel Workbook.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\testing\File Types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\wl_tests_files\wl_file_area\file_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8B4735-B8B7-48B8-B371-53FF1F1E2E1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB05B54-4F38-4C67-B480-B350A246451B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{756ADEE8-81A0-48F6-B77E-381A0BA5C0D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{756ADEE8-81A0-48F6-B77E-381A0BA5C0D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>C1</t>
   </si>
@@ -290,13 +290,43 @@
   </si>
   <si>
     <t>A1 &amp; B1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +339,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,8 +367,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,16 +698,16 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="A1:J10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,11 +730,11 @@
         <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -719,12 +761,12 @@
       <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
@@ -749,11 +791,11 @@
       <c r="I3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -781,11 +823,11 @@
       <c r="I4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,11 +855,11 @@
       <c r="I5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,11 +887,11 @@
       <c r="I6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,11 +919,11 @@
       <c r="I7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -909,11 +951,11 @@
       <c r="I8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -941,11 +983,11 @@
       <c r="I9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -973,8 +1015,8 @@
       <c r="I10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>84</v>
+      <c r="J10" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -982,6 +1024,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -992,434 +1035,426 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="str">
-        <f>Sheet1!A1 &amp; "(Sheet 2)"</f>
-        <v>A1 &amp; B1(Sheet 2)</v>
-      </c>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="str">
+        <f>Sheet1!A1</f>
+        <v>A1 &amp; B1</v>
+      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="1" t="str">
-        <f>Sheet1!C1 &amp; "(Sheet 2)"</f>
-        <v>C1(Sheet 2)</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <f>Sheet1!D1 &amp; "(Sheet 2)"</f>
-        <v>D1(Sheet 2)</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <f>Sheet1!E1 &amp; "(Sheet 2)"</f>
-        <v>E1(Sheet 2)</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <f>Sheet1!F1 &amp; "(Sheet 2)"</f>
-        <v>F1(Sheet 2)</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <f>Sheet1!G1 &amp; "(Sheet 2)"</f>
-        <v>G1(Sheet 2)</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <f>Sheet1!H1 &amp; "(Sheet 2)"</f>
-        <v>H1(Sheet 2)</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <f>Sheet1!I1 &amp; "(Sheet 2)"</f>
-        <v>I1(Sheet 2)</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <f>Sheet1!J1 &amp; "(Sheet 2)"</f>
-        <v>H1(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>Sheet1!A2 &amp; "(Sheet 2)"</f>
-        <v>A2 &amp; A3(Sheet 2)</v>
+        <f>Sheet1!C1</f>
+        <v>C1</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>Sheet1!D1</f>
+        <v>D1</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>Sheet1!E1</f>
+        <v>E1</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>Sheet1!F1</f>
+        <v>F1</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>Sheet1!G1</f>
+        <v>G1</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>Sheet1!H1</f>
+        <v>H1</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>Sheet1!I1</f>
+        <v>I1</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f>Sheet1!J1</f>
+        <v>J1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="str">
+        <f>Sheet1!A2</f>
+        <v>A2 &amp; A3</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>Sheet1!B2 &amp; "(Sheet 2)"</f>
-        <v>B2(Sheet 2)</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f>Sheet1!C2 &amp; "(Sheet 2)"</f>
-        <v>C2(Sheet 2)</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>Sheet1!D2 &amp; "(Sheet 2)"</f>
-        <v>D2(Sheet 2)</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>Sheet1!E2 &amp; "(Sheet 2)"</f>
-        <v>E2(Sheet 2)</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f>Sheet1!F2 &amp; "(Sheet 2)"</f>
-        <v>F2(Sheet 2)</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f>Sheet1!G2 &amp; "(Sheet 2)"</f>
-        <v>G2(Sheet 2)</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>Sheet1!H2 &amp; "(Sheet 2)"</f>
-        <v>H2(Sheet 2)</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>Sheet1!I2 &amp; "(Sheet 2)"</f>
-        <v>I2(Sheet 2)</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f>Sheet1!J2 &amp; "(Sheet 2)"</f>
-        <v>H2(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="str">
-        <f>Sheet1!B3 &amp; "(Sheet 2)"</f>
-        <v>B3(Sheet 2)</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f>Sheet1!C3 &amp; "(Sheet 2)"</f>
-        <v>C3(Sheet 2)</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>Sheet1!D3 &amp; "(Sheet 2)"</f>
-        <v>D3(Sheet 2)</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>Sheet1!E3 &amp; "(Sheet 2)"</f>
-        <v>E3(Sheet 2)</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f>Sheet1!F3 &amp; "(Sheet 2)"</f>
-        <v>F3(Sheet 2)</v>
-      </c>
-      <c r="G3" s="1" t="str">
-        <f>Sheet1!G3 &amp; "(Sheet 2)"</f>
-        <v>G3(Sheet 2)</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <f>Sheet1!H3 &amp; "(Sheet 2)"</f>
-        <v>H3(Sheet 2)</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f>Sheet1!I3 &amp; "(Sheet 2)"</f>
-        <v>I3(Sheet 2)</v>
-      </c>
-      <c r="J3" s="1" t="str">
-        <f>Sheet1!J3 &amp; "(Sheet 2)"</f>
-        <v>H3(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f>Sheet1!B2</f>
+        <v>B2</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>Sheet1!C2</f>
+        <v>C2</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>Sheet1!D2</f>
+        <v>D2</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>Sheet1!E2</f>
+        <v>E2</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>Sheet1!F2</f>
+        <v>F2</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>Sheet1!G2</f>
+        <v>G2</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>Sheet1!H2</f>
+        <v>H2</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>Sheet1!I2</f>
+        <v>I2</v>
+      </c>
+      <c r="J2" s="2" t="str">
+        <f>Sheet1!J2</f>
+        <v>J2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="str">
+        <f>Sheet1!B3</f>
+        <v>B3</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>Sheet1!C3</f>
+        <v>C3</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>Sheet1!D3</f>
+        <v>D3</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>Sheet1!E3</f>
+        <v>E3</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>Sheet1!F3</f>
+        <v>F3</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>Sheet1!G3</f>
+        <v>G3</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>Sheet1!H3</f>
+        <v>H3</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>Sheet1!I3</f>
+        <v>I3</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>Sheet1!J3</f>
+        <v>J3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
-        <f>Sheet1!A4 &amp; "(Sheet 2)"</f>
-        <v>A4(Sheet 2)</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>Sheet1!B4 &amp; "(Sheet 2)"</f>
-        <v>B4(Sheet 2)</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>Sheet1!C4 &amp; "(Sheet 2)"</f>
-        <v>C4(Sheet 2)</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>Sheet1!D4 &amp; "(Sheet 2)"</f>
-        <v>D4(Sheet 2)</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f>Sheet1!E4 &amp; "(Sheet 2)"</f>
-        <v>E4(Sheet 2)</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f>Sheet1!F4 &amp; "(Sheet 2)"</f>
-        <v>F4(Sheet 2)</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f>Sheet1!G4 &amp; "(Sheet 2)"</f>
-        <v>G4(Sheet 2)</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f>Sheet1!H4 &amp; "(Sheet 2)"</f>
-        <v>H4(Sheet 2)</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f>Sheet1!I4 &amp; "(Sheet 2)"</f>
-        <v>I4(Sheet 2)</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f>Sheet1!J4 &amp; "(Sheet 2)"</f>
-        <v>H4(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>Sheet1!A5 &amp; "(Sheet 2)"</f>
-        <v>A5(Sheet 2)</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f>Sheet1!B5 &amp; "(Sheet 2)"</f>
-        <v>B5(Sheet 2)</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <f>Sheet1!C5 &amp; "(Sheet 2)"</f>
-        <v>C5(Sheet 2)</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>Sheet1!D5 &amp; "(Sheet 2)"</f>
-        <v>D5(Sheet 2)</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f>Sheet1!E5 &amp; "(Sheet 2)"</f>
-        <v>E5(Sheet 2)</v>
-      </c>
-      <c r="F5" s="1" t="str">
-        <f>Sheet1!F5 &amp; "(Sheet 2)"</f>
-        <v>F5(Sheet 2)</v>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f>Sheet1!G5 &amp; "(Sheet 2)"</f>
-        <v>G5(Sheet 2)</v>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f>Sheet1!H5 &amp; "(Sheet 2)"</f>
-        <v>H5(Sheet 2)</v>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f>Sheet1!I5 &amp; "(Sheet 2)"</f>
-        <v>I5(Sheet 2)</v>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f>Sheet1!J5 &amp; "(Sheet 2)"</f>
-        <v>H5(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>Sheet1!A6 &amp; "(Sheet 2)"</f>
-        <v>A6(Sheet 2)</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f>Sheet1!B6 &amp; "(Sheet 2)"</f>
-        <v>B6(Sheet 2)</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f>Sheet1!C6 &amp; "(Sheet 2)"</f>
-        <v>C6(Sheet 2)</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>Sheet1!D6 &amp; "(Sheet 2)"</f>
-        <v>D6(Sheet 2)</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f>Sheet1!E6 &amp; "(Sheet 2)"</f>
-        <v>E6(Sheet 2)</v>
-      </c>
-      <c r="F6" s="1" t="str">
-        <f>Sheet1!F6 &amp; "(Sheet 2)"</f>
-        <v>F6(Sheet 2)</v>
-      </c>
-      <c r="G6" s="1" t="str">
-        <f>Sheet1!G6 &amp; "(Sheet 2)"</f>
-        <v>G6(Sheet 2)</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f>Sheet1!H6 &amp; "(Sheet 2)"</f>
-        <v>H6(Sheet 2)</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f>Sheet1!I6 &amp; "(Sheet 2)"</f>
-        <v>I6(Sheet 2)</v>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f>Sheet1!J6 &amp; "(Sheet 2)"</f>
-        <v>H6(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>Sheet1!A7 &amp; "(Sheet 2)"</f>
-        <v>A7(Sheet 2)</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>Sheet1!B7 &amp; "(Sheet 2)"</f>
-        <v>B7(Sheet 2)</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f>Sheet1!C7 &amp; "(Sheet 2)"</f>
-        <v>C7(Sheet 2)</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>Sheet1!D7 &amp; "(Sheet 2)"</f>
-        <v>D7(Sheet 2)</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f>Sheet1!E7 &amp; "(Sheet 2)"</f>
-        <v>E7(Sheet 2)</v>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f>Sheet1!F7 &amp; "(Sheet 2)"</f>
-        <v>F7(Sheet 2)</v>
-      </c>
-      <c r="G7" s="1" t="str">
-        <f>Sheet1!G7 &amp; "(Sheet 2)"</f>
-        <v>G7(Sheet 2)</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f>Sheet1!H7 &amp; "(Sheet 2)"</f>
-        <v>H7(Sheet 2)</v>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f>Sheet1!I7 &amp; "(Sheet 2)"</f>
-        <v>I7(Sheet 2)</v>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f>Sheet1!J7 &amp; "(Sheet 2)"</f>
-        <v>H7(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>Sheet1!A8 &amp; "(Sheet 2)"</f>
-        <v>A8(Sheet 2)</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f>Sheet1!B8 &amp; "(Sheet 2)"</f>
-        <v>B8(Sheet 2)</v>
-      </c>
-      <c r="C8" s="1" t="str">
-        <f>Sheet1!C8 &amp; "(Sheet 2)"</f>
-        <v>C8(Sheet 2)</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f>Sheet1!D8 &amp; "(Sheet 2)"</f>
-        <v>D8(Sheet 2)</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f>Sheet1!E8 &amp; "(Sheet 2)"</f>
-        <v>E8(Sheet 2)</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f>Sheet1!F8 &amp; "(Sheet 2)"</f>
-        <v>F8(Sheet 2)</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f>Sheet1!G8 &amp; "(Sheet 2)"</f>
-        <v>G8(Sheet 2)</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f>Sheet1!H8 &amp; "(Sheet 2)"</f>
-        <v>H8(Sheet 2)</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f>Sheet1!I8 &amp; "(Sheet 2)"</f>
-        <v>I8(Sheet 2)</v>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f>Sheet1!J8 &amp; "(Sheet 2)"</f>
-        <v>H8(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>Sheet1!A9 &amp; "(Sheet 2)"</f>
-        <v>A9(Sheet 2)</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>Sheet1!B9 &amp; "(Sheet 2)"</f>
-        <v>B9(Sheet 2)</v>
-      </c>
-      <c r="C9" s="1" t="str">
-        <f>Sheet1!C9 &amp; "(Sheet 2)"</f>
-        <v>C9(Sheet 2)</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f>Sheet1!D9 &amp; "(Sheet 2)"</f>
-        <v>D9(Sheet 2)</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f>Sheet1!E9 &amp; "(Sheet 2)"</f>
-        <v>E9(Sheet 2)</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f>Sheet1!F9 &amp; "(Sheet 2)"</f>
-        <v>F9(Sheet 2)</v>
-      </c>
-      <c r="G9" s="1" t="str">
-        <f>Sheet1!G9 &amp; "(Sheet 2)"</f>
-        <v>G9(Sheet 2)</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f>Sheet1!H9 &amp; "(Sheet 2)"</f>
-        <v>H9(Sheet 2)</v>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f>Sheet1!I9 &amp; "(Sheet 2)"</f>
-        <v>I9(Sheet 2)</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f>Sheet1!J9 &amp; "(Sheet 2)"</f>
-        <v>H9(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>Sheet1!A10 &amp; "(Sheet 2)"</f>
-        <v>A10(Sheet 2)</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f>Sheet1!B10 &amp; "(Sheet 2)"</f>
-        <v>B10(Sheet 2)</v>
-      </c>
-      <c r="C10" s="1" t="str">
-        <f>Sheet1!C10 &amp; "(Sheet 2)"</f>
-        <v>C10(Sheet 2)</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f>Sheet1!D10 &amp; "(Sheet 2)"</f>
-        <v>D10(Sheet 2)</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f>Sheet1!E10 &amp; "(Sheet 2)"</f>
-        <v>E10(Sheet 2)</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f>Sheet1!F10 &amp; "(Sheet 2)"</f>
-        <v>F10(Sheet 2)</v>
-      </c>
-      <c r="G10" s="1" t="str">
-        <f>Sheet1!G10 &amp; "(Sheet 2)"</f>
-        <v>G10(Sheet 2)</v>
-      </c>
-      <c r="H10" s="1" t="str">
-        <f>Sheet1!H10 &amp; "(Sheet 2)"</f>
-        <v>H10(Sheet 2)</v>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f>Sheet1!I10 &amp; "(Sheet 2)"</f>
-        <v>I10(Sheet 2)</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f>Sheet1!J10 &amp; "(Sheet 2)"</f>
-        <v>H10(Sheet 2)</v>
+        <f>Sheet1!A4</f>
+        <v>A4</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>Sheet1!B4</f>
+        <v>B4</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>Sheet1!C4</f>
+        <v>C4</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>Sheet1!D4</f>
+        <v>D4</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>Sheet1!E4</f>
+        <v>E4</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f>Sheet1!F4</f>
+        <v>F4</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>Sheet1!G4</f>
+        <v>G4</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>Sheet1!H4</f>
+        <v>H4</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>Sheet1!I4</f>
+        <v>I4</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f>Sheet1!J4</f>
+        <v>J4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="str">
+        <f>Sheet1!A5</f>
+        <v>A5</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>Sheet1!B5</f>
+        <v>B5</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>Sheet1!C5</f>
+        <v>C5</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>Sheet1!D5</f>
+        <v>D5</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>Sheet1!E5</f>
+        <v>E5</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>Sheet1!F5</f>
+        <v>F5</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f>Sheet1!G5</f>
+        <v>G5</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>Sheet1!H5</f>
+        <v>H5</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f>Sheet1!I5</f>
+        <v>I5</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f>Sheet1!J5</f>
+        <v>J5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="str">
+        <f>Sheet1!A6</f>
+        <v>A6</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>Sheet1!B6</f>
+        <v>B6</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>Sheet1!C6</f>
+        <v>C6</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>Sheet1!D6</f>
+        <v>D6</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>Sheet1!E6</f>
+        <v>E6</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f>Sheet1!F6</f>
+        <v>F6</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>Sheet1!G6</f>
+        <v>G6</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>Sheet1!H6</f>
+        <v>H6</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>Sheet1!I6</f>
+        <v>I6</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>Sheet1!J6</f>
+        <v>J6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="str">
+        <f>Sheet1!A7</f>
+        <v>A7</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>Sheet1!B7</f>
+        <v>B7</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>Sheet1!C7</f>
+        <v>C7</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>Sheet1!D7</f>
+        <v>D7</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>Sheet1!E7</f>
+        <v>E7</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f>Sheet1!F7</f>
+        <v>F7</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f>Sheet1!G7</f>
+        <v>G7</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>Sheet1!H7</f>
+        <v>H7</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f>Sheet1!I7</f>
+        <v>I7</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f>Sheet1!J7</f>
+        <v>J7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="str">
+        <f>Sheet1!A8</f>
+        <v>A8</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>Sheet1!B8</f>
+        <v>B8</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>Sheet1!C8</f>
+        <v>C8</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>Sheet1!D8</f>
+        <v>D8</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f>Sheet1!E8</f>
+        <v>E8</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f>Sheet1!F8</f>
+        <v>F8</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>Sheet1!G8</f>
+        <v>G8</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>Sheet1!H8</f>
+        <v>H8</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f>Sheet1!I8</f>
+        <v>I8</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>Sheet1!J8</f>
+        <v>J8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="str">
+        <f>Sheet1!A9</f>
+        <v>A9</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>Sheet1!B9</f>
+        <v>B9</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>Sheet1!C9</f>
+        <v>C9</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>Sheet1!D9</f>
+        <v>D9</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>Sheet1!E9</f>
+        <v>E9</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f>Sheet1!F9</f>
+        <v>F9</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f>Sheet1!G9</f>
+        <v>G9</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f>Sheet1!H9</f>
+        <v>H9</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>Sheet1!I9</f>
+        <v>I9</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f>Sheet1!J9</f>
+        <v>J9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="str">
+        <f>Sheet1!A10</f>
+        <v>A10</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>Sheet1!B10</f>
+        <v>B10</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>Sheet1!C10</f>
+        <v>C10</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>Sheet1!D10</f>
+        <v>D10</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f>Sheet1!E10</f>
+        <v>E10</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f>Sheet1!F10</f>
+        <v>F10</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f>Sheet1!G10</f>
+        <v>G10</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f>Sheet1!H10</f>
+        <v>H10</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f>Sheet1!I10</f>
+        <v>I10</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f>Sheet1!J10</f>
+        <v>J10</v>
       </c>
     </row>
   </sheetData>
@@ -1428,5 +1463,6 @@
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Menu: Update Preferences - Settings - General - Import
</commit_message>
<xml_diff>
--- a/src/wl_tests_files/wl_file_area/file_types/Excel Workbook.xlsx
+++ b/src/wl_tests_files/wl_file_area/file_types/Excel Workbook.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\testing\File Types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\wl_tests_files\wl_file_area\file_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8B4735-B8B7-48B8-B371-53FF1F1E2E1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB05B54-4F38-4C67-B480-B350A246451B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{756ADEE8-81A0-48F6-B77E-381A0BA5C0D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{756ADEE8-81A0-48F6-B77E-381A0BA5C0D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>C1</t>
   </si>
@@ -290,13 +290,43 @@
   </si>
   <si>
     <t>A1 &amp; B1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +339,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,8 +367,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,16 +698,16 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="A1:J10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,11 +730,11 @@
         <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -719,12 +761,12 @@
       <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
@@ -749,11 +791,11 @@
       <c r="I3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -781,11 +823,11 @@
       <c r="I4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,11 +855,11 @@
       <c r="I5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,11 +887,11 @@
       <c r="I6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,11 +919,11 @@
       <c r="I7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -909,11 +951,11 @@
       <c r="I8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -941,11 +983,11 @@
       <c r="I9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -973,8 +1015,8 @@
       <c r="I10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>84</v>
+      <c r="J10" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -982,6 +1024,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -992,434 +1035,426 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="str">
-        <f>Sheet1!A1 &amp; "(Sheet 2)"</f>
-        <v>A1 &amp; B1(Sheet 2)</v>
-      </c>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="str">
+        <f>Sheet1!A1</f>
+        <v>A1 &amp; B1</v>
+      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="1" t="str">
-        <f>Sheet1!C1 &amp; "(Sheet 2)"</f>
-        <v>C1(Sheet 2)</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <f>Sheet1!D1 &amp; "(Sheet 2)"</f>
-        <v>D1(Sheet 2)</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <f>Sheet1!E1 &amp; "(Sheet 2)"</f>
-        <v>E1(Sheet 2)</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <f>Sheet1!F1 &amp; "(Sheet 2)"</f>
-        <v>F1(Sheet 2)</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <f>Sheet1!G1 &amp; "(Sheet 2)"</f>
-        <v>G1(Sheet 2)</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <f>Sheet1!H1 &amp; "(Sheet 2)"</f>
-        <v>H1(Sheet 2)</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <f>Sheet1!I1 &amp; "(Sheet 2)"</f>
-        <v>I1(Sheet 2)</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <f>Sheet1!J1 &amp; "(Sheet 2)"</f>
-        <v>H1(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>Sheet1!A2 &amp; "(Sheet 2)"</f>
-        <v>A2 &amp; A3(Sheet 2)</v>
+        <f>Sheet1!C1</f>
+        <v>C1</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>Sheet1!D1</f>
+        <v>D1</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>Sheet1!E1</f>
+        <v>E1</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>Sheet1!F1</f>
+        <v>F1</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>Sheet1!G1</f>
+        <v>G1</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>Sheet1!H1</f>
+        <v>H1</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>Sheet1!I1</f>
+        <v>I1</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f>Sheet1!J1</f>
+        <v>J1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="str">
+        <f>Sheet1!A2</f>
+        <v>A2 &amp; A3</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>Sheet1!B2 &amp; "(Sheet 2)"</f>
-        <v>B2(Sheet 2)</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f>Sheet1!C2 &amp; "(Sheet 2)"</f>
-        <v>C2(Sheet 2)</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>Sheet1!D2 &amp; "(Sheet 2)"</f>
-        <v>D2(Sheet 2)</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>Sheet1!E2 &amp; "(Sheet 2)"</f>
-        <v>E2(Sheet 2)</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f>Sheet1!F2 &amp; "(Sheet 2)"</f>
-        <v>F2(Sheet 2)</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f>Sheet1!G2 &amp; "(Sheet 2)"</f>
-        <v>G2(Sheet 2)</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>Sheet1!H2 &amp; "(Sheet 2)"</f>
-        <v>H2(Sheet 2)</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>Sheet1!I2 &amp; "(Sheet 2)"</f>
-        <v>I2(Sheet 2)</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f>Sheet1!J2 &amp; "(Sheet 2)"</f>
-        <v>H2(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="str">
-        <f>Sheet1!B3 &amp; "(Sheet 2)"</f>
-        <v>B3(Sheet 2)</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f>Sheet1!C3 &amp; "(Sheet 2)"</f>
-        <v>C3(Sheet 2)</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>Sheet1!D3 &amp; "(Sheet 2)"</f>
-        <v>D3(Sheet 2)</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>Sheet1!E3 &amp; "(Sheet 2)"</f>
-        <v>E3(Sheet 2)</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f>Sheet1!F3 &amp; "(Sheet 2)"</f>
-        <v>F3(Sheet 2)</v>
-      </c>
-      <c r="G3" s="1" t="str">
-        <f>Sheet1!G3 &amp; "(Sheet 2)"</f>
-        <v>G3(Sheet 2)</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <f>Sheet1!H3 &amp; "(Sheet 2)"</f>
-        <v>H3(Sheet 2)</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f>Sheet1!I3 &amp; "(Sheet 2)"</f>
-        <v>I3(Sheet 2)</v>
-      </c>
-      <c r="J3" s="1" t="str">
-        <f>Sheet1!J3 &amp; "(Sheet 2)"</f>
-        <v>H3(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f>Sheet1!B2</f>
+        <v>B2</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>Sheet1!C2</f>
+        <v>C2</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>Sheet1!D2</f>
+        <v>D2</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>Sheet1!E2</f>
+        <v>E2</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>Sheet1!F2</f>
+        <v>F2</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>Sheet1!G2</f>
+        <v>G2</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>Sheet1!H2</f>
+        <v>H2</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>Sheet1!I2</f>
+        <v>I2</v>
+      </c>
+      <c r="J2" s="2" t="str">
+        <f>Sheet1!J2</f>
+        <v>J2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="str">
+        <f>Sheet1!B3</f>
+        <v>B3</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>Sheet1!C3</f>
+        <v>C3</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>Sheet1!D3</f>
+        <v>D3</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>Sheet1!E3</f>
+        <v>E3</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>Sheet1!F3</f>
+        <v>F3</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>Sheet1!G3</f>
+        <v>G3</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>Sheet1!H3</f>
+        <v>H3</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>Sheet1!I3</f>
+        <v>I3</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>Sheet1!J3</f>
+        <v>J3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
-        <f>Sheet1!A4 &amp; "(Sheet 2)"</f>
-        <v>A4(Sheet 2)</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>Sheet1!B4 &amp; "(Sheet 2)"</f>
-        <v>B4(Sheet 2)</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>Sheet1!C4 &amp; "(Sheet 2)"</f>
-        <v>C4(Sheet 2)</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>Sheet1!D4 &amp; "(Sheet 2)"</f>
-        <v>D4(Sheet 2)</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f>Sheet1!E4 &amp; "(Sheet 2)"</f>
-        <v>E4(Sheet 2)</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f>Sheet1!F4 &amp; "(Sheet 2)"</f>
-        <v>F4(Sheet 2)</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f>Sheet1!G4 &amp; "(Sheet 2)"</f>
-        <v>G4(Sheet 2)</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f>Sheet1!H4 &amp; "(Sheet 2)"</f>
-        <v>H4(Sheet 2)</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f>Sheet1!I4 &amp; "(Sheet 2)"</f>
-        <v>I4(Sheet 2)</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f>Sheet1!J4 &amp; "(Sheet 2)"</f>
-        <v>H4(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>Sheet1!A5 &amp; "(Sheet 2)"</f>
-        <v>A5(Sheet 2)</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f>Sheet1!B5 &amp; "(Sheet 2)"</f>
-        <v>B5(Sheet 2)</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <f>Sheet1!C5 &amp; "(Sheet 2)"</f>
-        <v>C5(Sheet 2)</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>Sheet1!D5 &amp; "(Sheet 2)"</f>
-        <v>D5(Sheet 2)</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f>Sheet1!E5 &amp; "(Sheet 2)"</f>
-        <v>E5(Sheet 2)</v>
-      </c>
-      <c r="F5" s="1" t="str">
-        <f>Sheet1!F5 &amp; "(Sheet 2)"</f>
-        <v>F5(Sheet 2)</v>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f>Sheet1!G5 &amp; "(Sheet 2)"</f>
-        <v>G5(Sheet 2)</v>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f>Sheet1!H5 &amp; "(Sheet 2)"</f>
-        <v>H5(Sheet 2)</v>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f>Sheet1!I5 &amp; "(Sheet 2)"</f>
-        <v>I5(Sheet 2)</v>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f>Sheet1!J5 &amp; "(Sheet 2)"</f>
-        <v>H5(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>Sheet1!A6 &amp; "(Sheet 2)"</f>
-        <v>A6(Sheet 2)</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f>Sheet1!B6 &amp; "(Sheet 2)"</f>
-        <v>B6(Sheet 2)</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f>Sheet1!C6 &amp; "(Sheet 2)"</f>
-        <v>C6(Sheet 2)</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>Sheet1!D6 &amp; "(Sheet 2)"</f>
-        <v>D6(Sheet 2)</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f>Sheet1!E6 &amp; "(Sheet 2)"</f>
-        <v>E6(Sheet 2)</v>
-      </c>
-      <c r="F6" s="1" t="str">
-        <f>Sheet1!F6 &amp; "(Sheet 2)"</f>
-        <v>F6(Sheet 2)</v>
-      </c>
-      <c r="G6" s="1" t="str">
-        <f>Sheet1!G6 &amp; "(Sheet 2)"</f>
-        <v>G6(Sheet 2)</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f>Sheet1!H6 &amp; "(Sheet 2)"</f>
-        <v>H6(Sheet 2)</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f>Sheet1!I6 &amp; "(Sheet 2)"</f>
-        <v>I6(Sheet 2)</v>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f>Sheet1!J6 &amp; "(Sheet 2)"</f>
-        <v>H6(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>Sheet1!A7 &amp; "(Sheet 2)"</f>
-        <v>A7(Sheet 2)</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>Sheet1!B7 &amp; "(Sheet 2)"</f>
-        <v>B7(Sheet 2)</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f>Sheet1!C7 &amp; "(Sheet 2)"</f>
-        <v>C7(Sheet 2)</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>Sheet1!D7 &amp; "(Sheet 2)"</f>
-        <v>D7(Sheet 2)</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f>Sheet1!E7 &amp; "(Sheet 2)"</f>
-        <v>E7(Sheet 2)</v>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f>Sheet1!F7 &amp; "(Sheet 2)"</f>
-        <v>F7(Sheet 2)</v>
-      </c>
-      <c r="G7" s="1" t="str">
-        <f>Sheet1!G7 &amp; "(Sheet 2)"</f>
-        <v>G7(Sheet 2)</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f>Sheet1!H7 &amp; "(Sheet 2)"</f>
-        <v>H7(Sheet 2)</v>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f>Sheet1!I7 &amp; "(Sheet 2)"</f>
-        <v>I7(Sheet 2)</v>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f>Sheet1!J7 &amp; "(Sheet 2)"</f>
-        <v>H7(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>Sheet1!A8 &amp; "(Sheet 2)"</f>
-        <v>A8(Sheet 2)</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f>Sheet1!B8 &amp; "(Sheet 2)"</f>
-        <v>B8(Sheet 2)</v>
-      </c>
-      <c r="C8" s="1" t="str">
-        <f>Sheet1!C8 &amp; "(Sheet 2)"</f>
-        <v>C8(Sheet 2)</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f>Sheet1!D8 &amp; "(Sheet 2)"</f>
-        <v>D8(Sheet 2)</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f>Sheet1!E8 &amp; "(Sheet 2)"</f>
-        <v>E8(Sheet 2)</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f>Sheet1!F8 &amp; "(Sheet 2)"</f>
-        <v>F8(Sheet 2)</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f>Sheet1!G8 &amp; "(Sheet 2)"</f>
-        <v>G8(Sheet 2)</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f>Sheet1!H8 &amp; "(Sheet 2)"</f>
-        <v>H8(Sheet 2)</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f>Sheet1!I8 &amp; "(Sheet 2)"</f>
-        <v>I8(Sheet 2)</v>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f>Sheet1!J8 &amp; "(Sheet 2)"</f>
-        <v>H8(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>Sheet1!A9 &amp; "(Sheet 2)"</f>
-        <v>A9(Sheet 2)</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>Sheet1!B9 &amp; "(Sheet 2)"</f>
-        <v>B9(Sheet 2)</v>
-      </c>
-      <c r="C9" s="1" t="str">
-        <f>Sheet1!C9 &amp; "(Sheet 2)"</f>
-        <v>C9(Sheet 2)</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f>Sheet1!D9 &amp; "(Sheet 2)"</f>
-        <v>D9(Sheet 2)</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f>Sheet1!E9 &amp; "(Sheet 2)"</f>
-        <v>E9(Sheet 2)</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f>Sheet1!F9 &amp; "(Sheet 2)"</f>
-        <v>F9(Sheet 2)</v>
-      </c>
-      <c r="G9" s="1" t="str">
-        <f>Sheet1!G9 &amp; "(Sheet 2)"</f>
-        <v>G9(Sheet 2)</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f>Sheet1!H9 &amp; "(Sheet 2)"</f>
-        <v>H9(Sheet 2)</v>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f>Sheet1!I9 &amp; "(Sheet 2)"</f>
-        <v>I9(Sheet 2)</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f>Sheet1!J9 &amp; "(Sheet 2)"</f>
-        <v>H9(Sheet 2)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>Sheet1!A10 &amp; "(Sheet 2)"</f>
-        <v>A10(Sheet 2)</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f>Sheet1!B10 &amp; "(Sheet 2)"</f>
-        <v>B10(Sheet 2)</v>
-      </c>
-      <c r="C10" s="1" t="str">
-        <f>Sheet1!C10 &amp; "(Sheet 2)"</f>
-        <v>C10(Sheet 2)</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f>Sheet1!D10 &amp; "(Sheet 2)"</f>
-        <v>D10(Sheet 2)</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f>Sheet1!E10 &amp; "(Sheet 2)"</f>
-        <v>E10(Sheet 2)</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f>Sheet1!F10 &amp; "(Sheet 2)"</f>
-        <v>F10(Sheet 2)</v>
-      </c>
-      <c r="G10" s="1" t="str">
-        <f>Sheet1!G10 &amp; "(Sheet 2)"</f>
-        <v>G10(Sheet 2)</v>
-      </c>
-      <c r="H10" s="1" t="str">
-        <f>Sheet1!H10 &amp; "(Sheet 2)"</f>
-        <v>H10(Sheet 2)</v>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f>Sheet1!I10 &amp; "(Sheet 2)"</f>
-        <v>I10(Sheet 2)</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f>Sheet1!J10 &amp; "(Sheet 2)"</f>
-        <v>H10(Sheet 2)</v>
+        <f>Sheet1!A4</f>
+        <v>A4</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>Sheet1!B4</f>
+        <v>B4</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>Sheet1!C4</f>
+        <v>C4</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>Sheet1!D4</f>
+        <v>D4</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>Sheet1!E4</f>
+        <v>E4</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f>Sheet1!F4</f>
+        <v>F4</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>Sheet1!G4</f>
+        <v>G4</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>Sheet1!H4</f>
+        <v>H4</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>Sheet1!I4</f>
+        <v>I4</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f>Sheet1!J4</f>
+        <v>J4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="str">
+        <f>Sheet1!A5</f>
+        <v>A5</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>Sheet1!B5</f>
+        <v>B5</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>Sheet1!C5</f>
+        <v>C5</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>Sheet1!D5</f>
+        <v>D5</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>Sheet1!E5</f>
+        <v>E5</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>Sheet1!F5</f>
+        <v>F5</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f>Sheet1!G5</f>
+        <v>G5</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>Sheet1!H5</f>
+        <v>H5</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f>Sheet1!I5</f>
+        <v>I5</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f>Sheet1!J5</f>
+        <v>J5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="str">
+        <f>Sheet1!A6</f>
+        <v>A6</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>Sheet1!B6</f>
+        <v>B6</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>Sheet1!C6</f>
+        <v>C6</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>Sheet1!D6</f>
+        <v>D6</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>Sheet1!E6</f>
+        <v>E6</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f>Sheet1!F6</f>
+        <v>F6</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>Sheet1!G6</f>
+        <v>G6</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>Sheet1!H6</f>
+        <v>H6</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>Sheet1!I6</f>
+        <v>I6</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>Sheet1!J6</f>
+        <v>J6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="str">
+        <f>Sheet1!A7</f>
+        <v>A7</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>Sheet1!B7</f>
+        <v>B7</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>Sheet1!C7</f>
+        <v>C7</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>Sheet1!D7</f>
+        <v>D7</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>Sheet1!E7</f>
+        <v>E7</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f>Sheet1!F7</f>
+        <v>F7</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f>Sheet1!G7</f>
+        <v>G7</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>Sheet1!H7</f>
+        <v>H7</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f>Sheet1!I7</f>
+        <v>I7</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f>Sheet1!J7</f>
+        <v>J7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="str">
+        <f>Sheet1!A8</f>
+        <v>A8</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>Sheet1!B8</f>
+        <v>B8</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>Sheet1!C8</f>
+        <v>C8</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>Sheet1!D8</f>
+        <v>D8</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f>Sheet1!E8</f>
+        <v>E8</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f>Sheet1!F8</f>
+        <v>F8</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>Sheet1!G8</f>
+        <v>G8</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>Sheet1!H8</f>
+        <v>H8</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f>Sheet1!I8</f>
+        <v>I8</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>Sheet1!J8</f>
+        <v>J8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="str">
+        <f>Sheet1!A9</f>
+        <v>A9</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>Sheet1!B9</f>
+        <v>B9</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>Sheet1!C9</f>
+        <v>C9</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>Sheet1!D9</f>
+        <v>D9</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>Sheet1!E9</f>
+        <v>E9</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f>Sheet1!F9</f>
+        <v>F9</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f>Sheet1!G9</f>
+        <v>G9</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f>Sheet1!H9</f>
+        <v>H9</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>Sheet1!I9</f>
+        <v>I9</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f>Sheet1!J9</f>
+        <v>J9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="str">
+        <f>Sheet1!A10</f>
+        <v>A10</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>Sheet1!B10</f>
+        <v>B10</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>Sheet1!C10</f>
+        <v>C10</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>Sheet1!D10</f>
+        <v>D10</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f>Sheet1!E10</f>
+        <v>E10</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f>Sheet1!F10</f>
+        <v>F10</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f>Sheet1!G10</f>
+        <v>G10</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f>Sheet1!H10</f>
+        <v>H10</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f>Sheet1!I10</f>
+        <v>I10</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f>Sheet1!J10</f>
+        <v>J10</v>
       </c>
     </row>
   </sheetData>
@@ -1428,5 +1463,6 @@
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>